<commit_message>
Lista entregables hito 3 actualizada
</commit_message>
<xml_diff>
--- a/Documentacion/Hito 3/Lista_de_Entregables_Hito_Tres.xlsx
+++ b/Documentacion/Hito 3/Lista_de_Entregables_Hito_Tres.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\Repositorio Sack\Documentacion\Hito 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
   <si>
     <t>Ordenados por Asignatura y Puntuacion</t>
   </si>
@@ -187,6 +187,48 @@
   </si>
   <si>
     <t>HORAS TOTATELS SIN CONTAR CON PD NI RV</t>
+  </si>
+  <si>
+    <t>Horas llevamos</t>
+  </si>
+  <si>
+    <t>falta estrategico</t>
+  </si>
+  <si>
+    <t>tu flipass</t>
+  </si>
+  <si>
+    <t>Fuera proyecto</t>
+  </si>
+  <si>
+    <t>Pasarlo a  SDL2</t>
+  </si>
+  <si>
+    <t>MiguelThings</t>
+  </si>
+  <si>
+    <t>BuenoPEroSiiQuehayniveles</t>
+  </si>
+  <si>
+    <t>Falta</t>
+  </si>
+  <si>
+    <t>Penalti</t>
+  </si>
+  <si>
+    <t>Visualización: visualizador OpenGL 4.X de las entidades tipo malla. Shader básicor. Con camaras y luces de varios tipos. Visualizacion con registro de camaras y luces</t>
+  </si>
+  <si>
+    <t>En tag hubo que rehacer arbol de escena y gestor de contenidos</t>
+  </si>
+  <si>
+    <t>20%  acabado</t>
+  </si>
+  <si>
+    <t>nada</t>
+  </si>
+  <si>
+    <t>bucea</t>
   </si>
 </sst>
 </file>
@@ -196,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]\-0.00;&quot;&quot;"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -246,12 +288,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF3FC8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -450,11 +486,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="11" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -471,7 +507,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="D32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -769,9 +807,10 @@
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="158.140625" customWidth="1"/>
+    <col min="4" max="4" width="169.85546875" customWidth="1"/>
     <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.140625" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="60">
@@ -811,7 +850,9 @@
       <c r="F5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="33" t="s">
+        <v>56</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:9">
@@ -827,7 +868,12 @@
       <c r="F6" s="14">
         <v>5</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="31">
+        <v>150</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9">
@@ -844,7 +890,12 @@
       <c r="F7" s="9">
         <v>6.36</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9">
@@ -861,7 +912,9 @@
       <c r="F8" s="9">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G8" s="30"/>
+      <c r="G8" s="30">
+        <v>0</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" ht="15">
@@ -878,8 +931,12 @@
       <c r="F9" s="9">
         <v>2.73</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="2"/>
+      <c r="G9" s="30">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="15">
       <c r="B10" s="19"/>
@@ -895,7 +952,9 @@
       <c r="F10" s="17">
         <v>3</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="30" t="s">
+        <v>59</v>
+      </c>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:9" ht="15">
@@ -912,7 +971,9 @@
       <c r="F11" s="17">
         <v>2</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="30" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:9" ht="15">
@@ -929,7 +990,9 @@
       <c r="F12" s="17">
         <v>1</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="30" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="13" spans="2:9" ht="15.75" customHeight="1">
       <c r="G13" s="30"/>
@@ -947,17 +1010,17 @@
       <c r="F16" s="1"/>
       <c r="G16" s="32"/>
     </row>
-    <row r="17" spans="3:7" ht="15.75" customHeight="1">
+    <row r="17" spans="3:8" ht="15.75" customHeight="1">
       <c r="D17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="32"/>
     </row>
-    <row r="18" spans="3:7" ht="15.75" customHeight="1">
+    <row r="18" spans="3:8" ht="15.75" customHeight="1">
       <c r="G18" s="32"/>
     </row>
-    <row r="19" spans="3:7" ht="15.75" customHeight="1">
+    <row r="19" spans="3:8" ht="15.75" customHeight="1">
       <c r="C19" s="5" t="s">
         <v>1</v>
       </c>
@@ -972,7 +1035,7 @@
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="3:7" ht="15.75" customHeight="1">
+    <row r="20" spans="3:8" ht="15.75" customHeight="1">
       <c r="C20" s="10" t="s">
         <v>5</v>
       </c>
@@ -987,7 +1050,7 @@
       </c>
       <c r="G20" s="31"/>
     </row>
-    <row r="21" spans="3:7" ht="15.75" customHeight="1">
+    <row r="21" spans="3:8" ht="15.75" customHeight="1">
       <c r="C21" s="10" t="s">
         <v>5</v>
       </c>
@@ -1000,9 +1063,14 @@
       <c r="F21" s="14">
         <v>5.45</v>
       </c>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G21" s="31">
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="15.75" customHeight="1">
       <c r="C22" s="7" t="s">
         <v>6</v>
       </c>
@@ -1015,9 +1083,14 @@
       <c r="F22" s="9">
         <v>5.45</v>
       </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G22" s="30">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="15.75" customHeight="1">
       <c r="C23" s="7" t="s">
         <v>6</v>
       </c>
@@ -1030,9 +1103,11 @@
       <c r="F23" s="9">
         <v>3.64</v>
       </c>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G23" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="15.75" customHeight="1">
       <c r="C24" s="7" t="s">
         <v>6</v>
       </c>
@@ -1045,9 +1120,11 @@
       <c r="F24" s="9">
         <v>1.82</v>
       </c>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G24" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="15.75" customHeight="1">
       <c r="C25" s="11" t="s">
         <v>9</v>
       </c>
@@ -1062,7 +1139,7 @@
       </c>
       <c r="G25" s="30"/>
     </row>
-    <row r="26" spans="3:7" ht="15.75" customHeight="1">
+    <row r="26" spans="3:8" ht="15.75" customHeight="1">
       <c r="C26" s="11" t="s">
         <v>9</v>
       </c>
@@ -1077,7 +1154,7 @@
       </c>
       <c r="G26" s="30"/>
     </row>
-    <row r="27" spans="3:7" ht="15.75" customHeight="1">
+    <row r="27" spans="3:8" ht="15.75" customHeight="1">
       <c r="C27" s="11" t="s">
         <v>9</v>
       </c>
@@ -1090,9 +1167,11 @@
       <c r="F27" s="16">
         <v>0.83299999999999996</v>
       </c>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G27" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="15.75" customHeight="1">
       <c r="C28" s="11" t="s">
         <v>9</v>
       </c>
@@ -1105,9 +1184,11 @@
       <c r="F28" s="16">
         <v>0.83299999999999996</v>
       </c>
-      <c r="G28" s="30"/>
-    </row>
-    <row r="29" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G28" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="15.75" customHeight="1">
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -1120,9 +1201,11 @@
       <c r="F29" s="16">
         <v>0.83299999999999996</v>
       </c>
-      <c r="G29" s="30"/>
-    </row>
-    <row r="30" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G29" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" ht="15.75" customHeight="1">
       <c r="C30" s="11" t="s">
         <v>9</v>
       </c>
@@ -1137,7 +1220,7 @@
       </c>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="3:7" ht="15.75" customHeight="1">
+    <row r="31" spans="3:8" ht="15.75" customHeight="1">
       <c r="C31" s="11" t="s">
         <v>9</v>
       </c>
@@ -1152,7 +1235,7 @@
       </c>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="3:7" ht="15.75" customHeight="1">
+    <row r="32" spans="3:8" ht="15.75" customHeight="1">
       <c r="C32" s="15" t="s">
         <v>7</v>
       </c>
@@ -1165,9 +1248,11 @@
       <c r="F32" s="17">
         <v>6</v>
       </c>
-      <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G32" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="15.75" customHeight="1">
       <c r="C33" s="15" t="s">
         <v>7</v>
       </c>
@@ -1180,9 +1265,11 @@
       <c r="F33" s="17">
         <v>2</v>
       </c>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G33" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="15.75" customHeight="1">
       <c r="C34" s="15" t="s">
         <v>7</v>
       </c>
@@ -1195,9 +1282,11 @@
       <c r="F34" s="17">
         <v>1</v>
       </c>
-      <c r="G34" s="30"/>
-    </row>
-    <row r="35" spans="3:7" ht="30">
+      <c r="G34" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" ht="30">
       <c r="C35" s="12" t="s">
         <v>11</v>
       </c>
@@ -1210,9 +1299,14 @@
       <c r="F35" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G35" s="33"/>
-    </row>
-    <row r="36" spans="3:7" ht="30">
+      <c r="G35" s="30">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="30">
       <c r="C36" s="12" t="s">
         <v>11</v>
       </c>
@@ -1225,9 +1319,11 @@
       <c r="F36" s="18">
         <v>2.6</v>
       </c>
-      <c r="G36" s="33"/>
-    </row>
-    <row r="37" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G36" s="30">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="15.75" customHeight="1">
       <c r="C37" s="12" t="s">
         <v>11</v>
       </c>
@@ -1240,9 +1336,11 @@
       <c r="F37" s="18">
         <v>1.6</v>
       </c>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G37" s="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" ht="15.75" customHeight="1">
       <c r="C38" s="12" t="s">
         <v>11</v>
       </c>
@@ -1255,9 +1353,11 @@
       <c r="F38" s="18">
         <v>1</v>
       </c>
-      <c r="G38" s="33"/>
-    </row>
-    <row r="39" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G38" s="30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" ht="15.75" customHeight="1">
       <c r="C39" s="12" t="s">
         <v>11</v>
       </c>
@@ -1270,9 +1370,11 @@
       <c r="F39" s="18">
         <v>1.6</v>
       </c>
-      <c r="G39" s="33"/>
-    </row>
-    <row r="40" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G39" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" ht="15.75" customHeight="1">
       <c r="C40" s="12" t="s">
         <v>11</v>
       </c>
@@ -1285,9 +1387,9 @@
       <c r="F40" s="18">
         <v>2.1</v>
       </c>
-      <c r="G40" s="33"/>
-    </row>
-    <row r="41" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="3:8" ht="15.75" customHeight="1">
       <c r="C41" s="12" t="s">
         <v>11</v>
       </c>
@@ -1300,14 +1402,14 @@
       <c r="F41" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G41" s="33"/>
-    </row>
-    <row r="42" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="3:8" ht="15.75" customHeight="1">
       <c r="C42" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="E42" s="18">
         <v>20</v>
@@ -1315,9 +1417,9 @@
       <c r="F42" s="18">
         <v>2.1</v>
       </c>
-      <c r="G42" s="33"/>
-    </row>
-    <row r="43" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" spans="3:8" ht="15.75" customHeight="1">
       <c r="C43" s="12" t="s">
         <v>11</v>
       </c>
@@ -1330,9 +1432,9 @@
       <c r="F43" s="18">
         <v>2.1</v>
       </c>
-      <c r="G43" s="33"/>
-    </row>
-    <row r="44" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" spans="3:8" ht="15.75" customHeight="1">
       <c r="C44" s="12" t="s">
         <v>11</v>
       </c>
@@ -1345,9 +1447,9 @@
       <c r="F44" s="18">
         <v>2.1</v>
       </c>
-      <c r="G44" s="33"/>
-    </row>
-    <row r="45" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="3:8" ht="15.75" customHeight="1">
       <c r="C45" s="12" t="s">
         <v>11</v>
       </c>
@@ -1360,9 +1462,9 @@
       <c r="F45" s="18">
         <v>2.6</v>
       </c>
-      <c r="G45" s="33"/>
-    </row>
-    <row r="46" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G45" s="30"/>
+    </row>
+    <row r="46" spans="3:8" ht="15.75" customHeight="1">
       <c r="C46" s="12" t="s">
         <v>11</v>
       </c>
@@ -1375,9 +1477,9 @@
       <c r="F46" s="18">
         <v>4.5</v>
       </c>
-      <c r="G46" s="33"/>
-    </row>
-    <row r="47" spans="3:7" ht="30">
+      <c r="G46" s="30"/>
+    </row>
+    <row r="47" spans="3:8" ht="30">
       <c r="C47" s="12" t="s">
         <v>11</v>
       </c>
@@ -1390,9 +1492,9 @@
       <c r="F47" s="18">
         <v>6.5</v>
       </c>
-      <c r="G47" s="33"/>
-    </row>
-    <row r="48" spans="3:7" ht="15.75" customHeight="1">
+      <c r="G47" s="30"/>
+    </row>
+    <row r="48" spans="3:8" ht="15.75" customHeight="1">
       <c r="C48" s="12" t="s">
         <v>11</v>
       </c>
@@ -1405,7 +1507,7 @@
       <c r="F48" s="18">
         <v>4.7</v>
       </c>
-      <c r="G48" s="33"/>
+      <c r="G48" s="30"/>
     </row>
     <row r="49" spans="3:7" ht="15.75" customHeight="1">
       <c r="C49" s="20" t="s">
@@ -1418,7 +1520,9 @@
       <c r="F49" s="27">
         <v>0.2</v>
       </c>
-      <c r="G49" s="30"/>
+      <c r="G49" s="30" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="50" spans="3:7" ht="15.75" customHeight="1">
       <c r="C50" s="20" t="s">
@@ -1431,7 +1535,9 @@
       <c r="F50" s="27">
         <v>0.15</v>
       </c>
-      <c r="G50" s="30"/>
+      <c r="G50" s="30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="51" spans="3:7" ht="15.75" customHeight="1">
       <c r="C51" s="20" t="s">
@@ -1444,7 +1550,9 @@
       <c r="F51" s="27">
         <v>0.05</v>
       </c>
-      <c r="G51" s="30"/>
+      <c r="G51" s="30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="52" spans="3:7" ht="15.75" customHeight="1">
       <c r="C52" s="20" t="s">
@@ -1457,7 +1565,9 @@
       <c r="F52" s="27">
         <v>0.1</v>
       </c>
-      <c r="G52" s="30"/>
+      <c r="G52" s="30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" customHeight="1">
       <c r="C53" s="22" t="s">
@@ -1470,7 +1580,9 @@
       <c r="F53" s="28">
         <v>0.2</v>
       </c>
-      <c r="G53" s="30"/>
+      <c r="G53" s="30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="54" spans="3:7" ht="15.75" customHeight="1">
       <c r="C54" s="22" t="s">
@@ -1483,7 +1595,9 @@
       <c r="F54" s="28">
         <v>0.2</v>
       </c>
-      <c r="G54" s="30"/>
+      <c r="G54" s="30" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="55" spans="3:7" ht="15.75" customHeight="1">
       <c r="C55" s="22" t="s">
@@ -1496,7 +1610,9 @@
       <c r="F55" s="28">
         <v>0.1</v>
       </c>
-      <c r="G55" s="30"/>
+      <c r="G55" s="30" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>